<commit_message>
Added charts to spreadsheet with textboxes
</commit_message>
<xml_diff>
--- a/data/brookings_paper_data.xlsx
+++ b/data/brookings_paper_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/Projects/real_time_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699C51E2-5229-CB49-80A9-B17D356590EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABCA294-563D-2646-B439-53A9429EBAB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2160" yWindow="820" windowWidth="38400" windowHeight="20460" activeTab="6" xr2:uid="{0DA6B4AB-4EC6-4C65-98B8-DB7914EF0FCB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="20460" activeTab="3" xr2:uid="{0DA6B4AB-4EC6-4C65-98B8-DB7914EF0FCB}"/>
   </bookViews>
   <sheets>
     <sheet name="figure1" sheetId="1" r:id="rId1"/>
@@ -377,6 +377,1173 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4941305B-346A-9447-8D49-DB4CE63BADC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="2044700"/>
+          <a:ext cx="6400800" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EBF600F-6CCA-1744-898D-611EC3A9E0A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11760200" y="1409700"/>
+          <a:ext cx="3022600" cy="431800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Figure 1: Early Policy Responses</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> to COVID-19</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>806450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6E8128D-22A8-D945-A046-6FBCB1CEBB33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1543050" y="5187950"/>
+          <a:ext cx="6400800" cy="5486400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1092200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EACFBD1-FB6F-9C49-98BE-73C0494634E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2832100" y="3098800"/>
+          <a:ext cx="3429000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Figure 2: Snapshots of Employment Data</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1054100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3600450" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8551081B-95F3-EE49-99ED-05AF34C51DB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2794000" y="3448050"/>
+          <a:ext cx="3600450" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Snapshots of Private Paid Employment</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1022350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3600450" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB834F26-A39B-3644-91A9-4B2A86C689F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762250" y="3784600"/>
+          <a:ext cx="3600450" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Snapshots of Leisure and Hospitality Employment</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1041400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3600450" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B94B9E9-09AF-2443-9D4A-0F231708CAEE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2781300" y="4260850"/>
+          <a:ext cx="3600450" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Note: Paid employment</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>996950</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3600450" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF94D017-2771-A74E-9425-114DA0A7B61B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2736850" y="4546600"/>
+          <a:ext cx="3600450" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Source: Staff calculations;</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> ADP, LLP; Bureau of Labor Statistics</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BC3B684-5747-694A-90A9-F6416724763E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10541000" y="1422400"/>
+          <a:ext cx="4165600" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Figure 3: Snapshots of Consumer Spending (percent change from same period in 2019)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4992360-B928-0041-B63B-F8A25EB093EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10541000" y="2032000"/>
+          <a:ext cx="3797300" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Note: 7-day</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> averages.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F77361B-756A-F54C-9C25-D612C3B721E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10464800" y="2692400"/>
+          <a:ext cx="3797300" cy="495300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Source: Census Bureau,  Fiserv, OpenTable, TSA.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA0E631E-E2E3-0F46-AE42-AABED2B5592D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10515600" y="3289300"/>
+          <a:ext cx="5257800" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3259B396-D1F5-3E4D-B671-A2360090B1B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6997700" y="3530600"/>
+          <a:ext cx="4114800" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8849A453-F655-CA4E-9D0F-B256CC450E47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6870700" y="1244600"/>
+          <a:ext cx="3949700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Figure 4: ADP and BLS Measures of Employment</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FB9402E-D5EA-EA45-A87E-488F39101D27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6870700" y="1714500"/>
+          <a:ext cx="3949700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Note: Paid employment.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E402E571-F282-0846-8B16-670F61A57599}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6870700" y="2476500"/>
+          <a:ext cx="3949700" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Source: Staff calculations, ADP, LLP, Bureau of Labor Statistics.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F155154-5549-3B43-96CE-16B38B6FDF90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5969000" y="1651000"/>
+          <a:ext cx="4114800" cy="3657600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -677,7 +1844,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -910,6 +2077,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -19210,8 +20378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F5501A1-D6A5-4527-9576-D50669031A5A}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView topLeftCell="B21" zoomScale="200" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19420,6 +20588,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -19428,7 +20597,7 @@
   <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21241,6 +22410,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -21248,8 +22418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A87A70A-8C8E-492B-8C05-7DA78F243F2D}">
   <dimension ref="A1:E90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22368,6 +23538,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -23742,6 +24913,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -23929,7 +25101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50786F96-A219-44A9-B14C-0D75E6D83E48}">
   <dimension ref="A1:E95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>